<commit_message>
sidebar change and dashboard
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Team Outlier\lifeline_streamlit\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377607C4-E9DA-460E-BE9F-61D6FCB9BE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B6FEE2-2C74-4136-AEA5-64C0DF47F5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D2D4F83-4A06-4352-86C3-493D727EC95E}"/>
   </bookViews>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FD6DC2-4418-4402-AA17-6229F227E603}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2700,7 +2700,7 @@
         <v>1.05E+16</v>
       </c>
       <c r="D19">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -3407,7 +3407,7 @@
         <v>1.05E+16</v>
       </c>
       <c r="D26">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="E26">
         <v>1</v>

</xml_diff>